<commit_message>
Updated diagrams and bom
made diagram more detailed, added SRAM and a few more buffers to the
bill of materials
</commit_message>
<xml_diff>
--- a/Lab2/Bill_of_materials.xlsx
+++ b/Lab2/Bill_of_materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgma2010\ee478\Lab2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rynmcd\Documents\GitHub\ee478\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Part No</t>
   </si>
@@ -104,16 +104,19 @@
     <t>haveit ?</t>
   </si>
   <si>
-    <t>Goat</t>
-  </si>
-  <si>
-    <t>Because smoke demons</t>
-  </si>
-  <si>
     <t>Resistors</t>
   </si>
   <si>
     <t>Capacitors</t>
+  </si>
+  <si>
+    <t>SRAM</t>
+  </si>
+  <si>
+    <t>Store measurment data</t>
+  </si>
+  <si>
+    <t>have them</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +530,7 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -563,20 +566,26 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done with phase 1
</commit_message>
<xml_diff>
--- a/Lab2/Bill_of_materials.xlsx
+++ b/Lab2/Bill_of_materials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Part No</t>
   </si>
@@ -44,27 +44,12 @@
     <t>Price</t>
   </si>
   <si>
-    <t>5VDC motor</t>
-  </si>
-  <si>
-    <t>PIC18F452</t>
-  </si>
-  <si>
     <t>40-pin PIC microcontroller</t>
   </si>
   <si>
     <t>Xtal Oscillator</t>
   </si>
   <si>
-    <t>TIP22</t>
-  </si>
-  <si>
-    <t>Mosfet</t>
-  </si>
-  <si>
-    <t>Motor driver</t>
-  </si>
-  <si>
     <t>nodes/controller</t>
   </si>
   <si>
@@ -74,12 +59,6 @@
     <t>GALs</t>
   </si>
   <si>
-    <t>Lots of Wires</t>
-  </si>
-  <si>
-    <t>infinity</t>
-  </si>
-  <si>
     <t>UART-rs232 level shifter</t>
   </si>
   <si>
@@ -95,31 +74,67 @@
     <t>EE store</t>
   </si>
   <si>
-    <t>have it</t>
-  </si>
-  <si>
-    <t>haveit ?</t>
-  </si>
-  <si>
-    <t>Resistors</t>
-  </si>
-  <si>
-    <t>Capacitors</t>
-  </si>
-  <si>
     <t>SRAM</t>
   </si>
   <si>
     <t>Store measurment data</t>
   </si>
   <si>
-    <t>have them</t>
-  </si>
-  <si>
     <t>CY7C128A</t>
   </si>
   <si>
     <t>OSC-20MHZ</t>
+  </si>
+  <si>
+    <t>GAL22v10-25LP</t>
+  </si>
+  <si>
+    <t>PIC18F25K22-I/SP</t>
+  </si>
+  <si>
+    <t>I2C pull ups</t>
+  </si>
+  <si>
+    <t>CF18JT4K70</t>
+  </si>
+  <si>
+    <t>Resistor, 4.7k ohm +/-5%, 1/8W</t>
+  </si>
+  <si>
+    <t>Resistor, 10k ohm, +/- 5%, 1/8W</t>
+  </si>
+  <si>
+    <t>pull ups</t>
+  </si>
+  <si>
+    <t>CF18JT510K</t>
+  </si>
+  <si>
+    <t>Capacitors, 1uF, 50V</t>
+  </si>
+  <si>
+    <t>bypass and level shift</t>
+  </si>
+  <si>
+    <t>UPJ1H010MDD1TD</t>
+  </si>
+  <si>
+    <t>Switch, SPDT</t>
+  </si>
+  <si>
+    <t>System reset</t>
+  </si>
+  <si>
+    <t>25136NAH</t>
+  </si>
+  <si>
+    <t>system clock</t>
+  </si>
+  <si>
+    <t>Custom circuit board(3)</t>
+  </si>
+  <si>
+    <t>oshpark</t>
   </si>
 </sst>
 </file>
@@ -445,13 +460,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -477,132 +492,175 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.96</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*C2</f>
-        <v>0</v>
+        <f t="shared" ref="F2:F11" si="0">E2*C2</f>
+        <v>5.92</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.4</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F11" si="0">E3*C3</f>
-        <v>0</v>
+        <f>E3*C3</f>
+        <v>4.8</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
       <c r="E4" s="1">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>4.8</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="E5" s="1">
+        <v>0.75</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.95</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1" t="e">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0.16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.09</v>
       </c>
       <c r="F8" s="1">
-        <v>0.74</v>
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -610,38 +668,65 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.3</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.1000000000000001</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>20</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Done with phase 1"
This reverts commit cc6a0e2afad81a55f63c8c3983d7b3299cb41fbd.
</commit_message>
<xml_diff>
--- a/Lab2/Bill_of_materials.xlsx
+++ b/Lab2/Bill_of_materials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Part No</t>
   </si>
@@ -44,12 +44,27 @@
     <t>Price</t>
   </si>
   <si>
+    <t>5VDC motor</t>
+  </si>
+  <si>
+    <t>PIC18F452</t>
+  </si>
+  <si>
     <t>40-pin PIC microcontroller</t>
   </si>
   <si>
     <t>Xtal Oscillator</t>
   </si>
   <si>
+    <t>TIP22</t>
+  </si>
+  <si>
+    <t>Mosfet</t>
+  </si>
+  <si>
+    <t>Motor driver</t>
+  </si>
+  <si>
     <t>nodes/controller</t>
   </si>
   <si>
@@ -59,6 +74,12 @@
     <t>GALs</t>
   </si>
   <si>
+    <t>Lots of Wires</t>
+  </si>
+  <si>
+    <t>infinity</t>
+  </si>
+  <si>
     <t>UART-rs232 level shifter</t>
   </si>
   <si>
@@ -74,67 +95,31 @@
     <t>EE store</t>
   </si>
   <si>
+    <t>have it</t>
+  </si>
+  <si>
+    <t>haveit ?</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
     <t>SRAM</t>
   </si>
   <si>
     <t>Store measurment data</t>
   </si>
   <si>
+    <t>have them</t>
+  </si>
+  <si>
     <t>CY7C128A</t>
   </si>
   <si>
     <t>OSC-20MHZ</t>
-  </si>
-  <si>
-    <t>GAL22v10-25LP</t>
-  </si>
-  <si>
-    <t>PIC18F25K22-I/SP</t>
-  </si>
-  <si>
-    <t>I2C pull ups</t>
-  </si>
-  <si>
-    <t>CF18JT4K70</t>
-  </si>
-  <si>
-    <t>Resistor, 4.7k ohm +/-5%, 1/8W</t>
-  </si>
-  <si>
-    <t>Resistor, 10k ohm, +/- 5%, 1/8W</t>
-  </si>
-  <si>
-    <t>pull ups</t>
-  </si>
-  <si>
-    <t>CF18JT510K</t>
-  </si>
-  <si>
-    <t>Capacitors, 1uF, 50V</t>
-  </si>
-  <si>
-    <t>bypass and level shift</t>
-  </si>
-  <si>
-    <t>UPJ1H010MDD1TD</t>
-  </si>
-  <si>
-    <t>Switch, SPDT</t>
-  </si>
-  <si>
-    <t>System reset</t>
-  </si>
-  <si>
-    <t>25136NAH</t>
-  </si>
-  <si>
-    <t>system clock</t>
-  </si>
-  <si>
-    <t>Custom circuit board(3)</t>
-  </si>
-  <si>
-    <t>oshpark</t>
   </si>
 </sst>
 </file>
@@ -460,13 +445,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -492,175 +477,132 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2.96</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F11" si="0">E2*C2</f>
-        <v>5.92</v>
+        <f>E2*C2</f>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2.4</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*C3</f>
-        <v>4.8</v>
+        <f t="shared" ref="F3:F11" si="0">E3*C3</f>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" s="1">
-        <v>3.5</v>
+        <v>2.4</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4.8</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.75</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
       <c r="C6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1.95</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>3.9</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="F7" s="1">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>0.16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.09</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
+        <v>0.74</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,65 +610,38 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.3</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
       <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1.1000000000000001</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>